<commit_message>
Fix Excel template filename typo
</commit_message>
<xml_diff>
--- a/prediction_model/data/Feedback_Dashboard_Template..xlsx
+++ b/prediction_model/data/Feedback_Dashboard_Template..xlsx
@@ -5,28 +5,29 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abiod\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abiod\Documents\GitHub\scratch\prediction_model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F32FD4E-BBE8-40CA-9EC0-8B3D46650926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B3C5D5-5714-44A4-B1A7-5351542A6DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="18000" windowHeight="9210" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="9" r:id="rId1"/>
-    <sheet name="Feedback_Data" sheetId="1" r:id="rId2"/>
-    <sheet name="Dashboard1" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="8" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId8"/>
-    <sheet name="Pi" sheetId="4" r:id="rId9"/>
+    <sheet name="Output" sheetId="10" r:id="rId2"/>
+    <sheet name="Feedback_Data" sheetId="1" r:id="rId3"/>
+    <sheet name="Dashboard1" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId9"/>
+    <sheet name="Pi" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId10"/>
-    <pivotCache cacheId="1" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="109">
   <si>
     <t>Date</t>
   </si>
@@ -320,6 +321,57 @@
   <si>
     <t>&lt;1/1/2025</t>
   </si>
+  <si>
+    <t>Sentiment Score</t>
+  </si>
+  <si>
+    <t>Risk Level</t>
+  </si>
+  <si>
+    <t>Top Issue Summary</t>
+  </si>
+  <si>
+    <t>Recommendation</t>
+  </si>
+  <si>
+    <t>Probability Score</t>
+  </si>
+  <si>
+    <t>Last Updated</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>No specific issues identified</t>
+  </si>
+  <si>
+    <t>Immediate maintenance required for ATM network. Check for hardware failures and cash availability.</t>
+  </si>
+  <si>
+    <t>Immediate investigation required. Escalate to senior management and deploy dedicated resources.</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>slow slow slow slow slow slow slow slow slow slow</t>
+  </si>
+  <si>
+    <t>Improve follow-up process and monitor trends closely. Schedule review within 2 weeks.</t>
+  </si>
+  <si>
+    <t>Stable</t>
+  </si>
+  <si>
+    <t>crash crash crash crash crash crash crash crash crash crash</t>
+  </si>
+  <si>
+    <t>Online banking service running smoothly. Monitor for security threats.</t>
+  </si>
+  <si>
+    <t>Continue current monitoring practices. Maintain quality standards.</t>
+  </si>
 </sst>
 </file>
 
@@ -328,7 +380,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,8 +393,16 @@
       <sz val="16"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +412,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEAEAEA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -384,6 +450,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -26447,9 +26515,9 @@
       <selection activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="6"/>
+    <col min="1" max="16384" width="8.7109375" style="6"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26457,28 +26525,305 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{591811CE-B39F-48D6-9832-E84C075766CE}">
+  <dimension ref="A3:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D54640-4295-4469-A699-391B94CAFA58}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="93" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>0.75</v>
+      </c>
+      <c r="I2" s="9">
+        <v>46004.285381944443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3">
+        <v>0.625</v>
+      </c>
+      <c r="I3" s="9">
+        <v>46004.285381944443</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>-0.30000000000000004</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="I4" s="9">
+        <v>46004.285381944443</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5">
+        <v>0.375</v>
+      </c>
+      <c r="I5" s="9">
+        <v>46004.285381944443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0.8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6">
+        <v>4.9999999999999989E-2</v>
+      </c>
+      <c r="I6" s="9">
+        <v>46004.285381944443</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+    <sheetView zoomScale="98" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="1"/>
-    <col min="6" max="6" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -26507,7 +26852,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45658</v>
       </c>
@@ -26537,7 +26882,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45659</v>
       </c>
@@ -26567,7 +26912,7 @@
         <v>0.58823529411764708</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45660</v>
       </c>
@@ -26597,7 +26942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45661</v>
       </c>
@@ -26627,7 +26972,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45662</v>
       </c>
@@ -26650,7 +26995,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45663</v>
       </c>
@@ -26673,7 +27018,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45664</v>
       </c>
@@ -26696,7 +27041,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45665</v>
       </c>
@@ -26719,7 +27064,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45666</v>
       </c>
@@ -26742,7 +27087,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45667</v>
       </c>
@@ -26765,7 +27110,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45668</v>
       </c>
@@ -26788,7 +27133,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45669</v>
       </c>
@@ -26811,7 +27156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45670</v>
       </c>
@@ -26834,7 +27179,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45671</v>
       </c>
@@ -26857,7 +27202,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45672</v>
       </c>
@@ -26880,7 +27225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45673</v>
       </c>
@@ -26903,7 +27248,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45674</v>
       </c>
@@ -26926,7 +27271,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45675</v>
       </c>
@@ -26949,7 +27294,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45676</v>
       </c>
@@ -26972,7 +27317,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45677</v>
       </c>
@@ -26995,7 +27340,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45678</v>
       </c>
@@ -27018,7 +27363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45679</v>
       </c>
@@ -27041,7 +27386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45680</v>
       </c>
@@ -27064,7 +27409,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45681</v>
       </c>
@@ -27087,7 +27432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45682</v>
       </c>
@@ -27110,7 +27455,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45683</v>
       </c>
@@ -27133,7 +27478,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45684</v>
       </c>
@@ -27156,7 +27501,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45685</v>
       </c>
@@ -27179,7 +27524,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45686</v>
       </c>
@@ -27202,7 +27547,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45687</v>
       </c>
@@ -27225,7 +27570,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45688</v>
       </c>
@@ -27248,7 +27593,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45689</v>
       </c>
@@ -27271,7 +27616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>45690</v>
       </c>
@@ -27294,7 +27639,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>45691</v>
       </c>
@@ -27317,7 +27662,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>45692</v>
       </c>
@@ -27340,7 +27685,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>45693</v>
       </c>
@@ -27363,7 +27708,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>45694</v>
       </c>
@@ -27386,7 +27731,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>45695</v>
       </c>
@@ -27409,7 +27754,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>45696</v>
       </c>
@@ -27432,7 +27777,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>45697</v>
       </c>
@@ -27455,7 +27800,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45698</v>
       </c>
@@ -27478,7 +27823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45699</v>
       </c>
@@ -27501,7 +27846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>45700</v>
       </c>
@@ -27524,7 +27869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45701</v>
       </c>
@@ -27547,7 +27892,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45702</v>
       </c>
@@ -27570,7 +27915,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45703</v>
       </c>
@@ -27593,7 +27938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45704</v>
       </c>
@@ -27616,7 +27961,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45705</v>
       </c>
@@ -27639,7 +27984,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>45706</v>
       </c>
@@ -27662,7 +28007,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>45707</v>
       </c>
@@ -27694,7 +28039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="P10"/>
   <sheetViews>
@@ -27702,9 +28047,9 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="10" spans="16:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P10" t="s">
         <v>90</v>
       </c>
@@ -27715,7 +28060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1155A662-7BF5-4680-92FB-AA13B06AE516}">
   <dimension ref="A3:G10"/>
   <sheetViews>
@@ -27723,15 +28068,15 @@
       <selection activeCell="A3" sqref="A3:G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="2.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>85</v>
       </c>
@@ -27739,7 +28084,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>81</v>
       </c>
@@ -27762,7 +28107,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -27773,7 +28118,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -27784,7 +28129,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -27795,7 +28140,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -27806,7 +28151,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -27817,7 +28162,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>83</v>
       </c>
@@ -27846,7 +28191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD248094-975F-493C-8312-B6FA907BA9A5}">
   <dimension ref="A3:E11"/>
   <sheetViews>
@@ -27854,16 +28199,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -27871,7 +28216,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>81</v>
       </c>
@@ -27888,7 +28233,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -27899,7 +28244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -27910,7 +28255,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -27921,7 +28266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -27932,7 +28277,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -27943,12 +28288,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>83</v>
       </c>
@@ -27967,7 +28312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{095BC04F-660D-4125-B406-9D845FBC3A12}">
   <dimension ref="A3:B7"/>
   <sheetViews>
@@ -27975,14 +28320,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>81</v>
       </c>
@@ -27990,12 +28335,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>87</v>
       </c>
@@ -28003,7 +28348,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>88</v>
       </c>
@@ -28011,88 +28356,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B7">
         <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28A343A-750F-4C93-8C03-799623657612}">
-  <dimension ref="A3:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9">
-        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -28102,6 +28371,82 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28A343A-750F-4C93-8C03-799623657612}">
+  <dimension ref="A3:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC53BD98-F8D5-4041-B2A8-08B963DD0A7D}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -28109,13 +28454,13 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>71</v>
       </c>
@@ -28124,7 +28469,7 @@
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -28133,7 +28478,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -28142,7 +28487,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -28151,7 +28496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -28167,85 +28512,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{591811CE-B39F-48D6-9832-E84C075766CE}">
-  <dimension ref="A3:B10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Excel file path to correct filename
</commit_message>
<xml_diff>
--- a/prediction_model/data/Feedback_Dashboard_Template..xlsx
+++ b/prediction_model/data/Feedback_Dashboard_Template..xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abiod\Documents\GitHub\scratch\prediction_model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B3C5D5-5714-44A4-B1A7-5351542A6DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F98E929-1B12-489F-B8D0-0EDE307A9CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="18000" windowHeight="9210" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26678,7 +26678,7 @@
         <v>0.75</v>
       </c>
       <c r="I2" s="9">
-        <v>46004.285381944443</v>
+        <v>46004.303194444445</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -26707,7 +26707,7 @@
         <v>0.625</v>
       </c>
       <c r="I3" s="9">
-        <v>46004.285381944443</v>
+        <v>46004.303194444445</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -26736,7 +26736,7 @@
         <v>0.57499999999999996</v>
       </c>
       <c r="I4" s="9">
-        <v>46004.285381944443</v>
+        <v>46004.303194444445</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -26765,7 +26765,7 @@
         <v>0.375</v>
       </c>
       <c r="I5" s="9">
-        <v>46004.285381944443</v>
+        <v>46004.303194444445</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -26794,7 +26794,7 @@
         <v>4.9999999999999989E-2</v>
       </c>
       <c r="I6" s="9">
-        <v>46004.285381944443</v>
+        <v>46004.303194444445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>